<commit_message>
Robot + objectif + todo
</commit_message>
<xml_diff>
--- a/planches/tableaux_num.xlsx
+++ b/planches/tableaux_num.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauth\Documents\Gauthier\ISEP\A1\Cours\Algo_Prog\Ricochet-Robot\planches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72220FDF-B669-432C-AAF6-BF2F6420ECD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0CA6A9-319F-4D27-9345-39BD823D329C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7270" xr2:uid="{FD5C230A-77F0-4B06-9831-CBC9F5573B23}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FD5C230A-77F0-4B06-9831-CBC9F5573B23}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4F93EE-E3AD-40CD-80C6-0C607FDE4CD1}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>